<commit_message>
Added Plug 6 - Gui adjustments
</commit_message>
<xml_diff>
--- a/Plug1_data.xlsx
+++ b/Plug1_data.xlsx
@@ -3392,10 +3392,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="354">
-                  <c:v>0</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="355">
-                  <c:v>0</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="356">
                   <c:v>0</c:v>
@@ -7722,10 +7722,10 @@
         <v>357</v>
       </c>
       <c r="B356">
-        <v>0</v>
+        <v>0.46</v>
       </c>
       <c r="C356">
-        <v>0</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="357" spans="1:3">
@@ -7733,10 +7733,10 @@
         <v>358</v>
       </c>
       <c r="B357">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="C357">
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="358" spans="1:3">

</xml_diff>